<commit_message>
removed israel from map
</commit_message>
<xml_diff>
--- a/Examples/Coordinates.xlsx
+++ b/Examples/Coordinates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Country</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Israel</t>
   </si>
   <si>
     <t>United Kingdom of Great Britain and Northern Ireland</t>
@@ -513,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -563,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,7 +574,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,12 +588,12 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -605,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +686,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -703,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -717,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -731,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -745,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -759,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -773,102 +770,102 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>45</v>
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
+      <c r="A23" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>43</v>
+      <c r="A24" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>44</v>
@@ -876,125 +873,125 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>6</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
         <v>44</v>
@@ -1002,100 +999,86 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>